<commit_message>
Changed "Analyse" to "Corti"
</commit_message>
<xml_diff>
--- a/Output/Cortisol.xlsx
+++ b/Output/Cortisol.xlsx
@@ -370,22 +370,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Analyse_1</t>
+          <t>Corti1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Analyse_2</t>
+          <t>Corti2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Analyse_3</t>
+          <t>Corti3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Analyse_4</t>
+          <t>Corti4</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
New cortisol analyses 02/03/2021
</commit_message>
<xml_diff>
--- a/Output/Cortisol.xlsx
+++ b/Output/Cortisol.xlsx
@@ -552,6 +552,18 @@
           <t>ZaHa</t>
         </is>
       </c>
+      <c r="C9">
+        <v>0.04</v>
+      </c>
+      <c r="D9">
+        <v>0.03</v>
+      </c>
+      <c r="E9">
+        <v>0.02</v>
+      </c>
+      <c r="F9">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -1002,6 +1014,18 @@
           <t>Brse</t>
         </is>
       </c>
+      <c r="C30">
+        <v>0.33</v>
+      </c>
+      <c r="D30">
+        <v>0.28</v>
+      </c>
+      <c r="E30">
+        <v>0.1</v>
+      </c>
+      <c r="F30">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -1594,6 +1618,12 @@
           <t>MonChri</t>
         </is>
       </c>
+      <c r="C58">
+        <v>0.17</v>
+      </c>
+      <c r="D58">
+        <v>0.21</v>
+      </c>
       <c r="E58">
         <v>0.23</v>
       </c>
@@ -1654,6 +1684,18 @@
           <t>HabCha</t>
         </is>
       </c>
+      <c r="C61">
+        <v>0.12</v>
+      </c>
+      <c r="D61">
+        <v>0.11</v>
+      </c>
+      <c r="E61">
+        <v>0.11</v>
+      </c>
+      <c r="F61">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -1664,6 +1706,18 @@
           <t>BoucIli</t>
         </is>
       </c>
+      <c r="C62">
+        <v>0.1</v>
+      </c>
+      <c r="D62">
+        <v>0.12</v>
+      </c>
+      <c r="E62">
+        <v>0.11</v>
+      </c>
+      <c r="F62">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -1674,6 +1728,18 @@
           <t>DaiAnt</t>
         </is>
       </c>
+      <c r="C63">
+        <v>0.26</v>
+      </c>
+      <c r="D63">
+        <v>0.22</v>
+      </c>
+      <c r="E63">
+        <v>0.24</v>
+      </c>
+      <c r="F63">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -1788,6 +1854,18 @@
           <t>DIEAL</t>
         </is>
       </c>
+      <c r="C72">
+        <v>0.19</v>
+      </c>
+      <c r="D72">
+        <v>0.08</v>
+      </c>
+      <c r="E72">
+        <v>0.06</v>
+      </c>
+      <c r="F72">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -1798,6 +1876,18 @@
           <t>SHEAY</t>
         </is>
       </c>
+      <c r="C73">
+        <v>0.02</v>
+      </c>
+      <c r="D73">
+        <v>0.09</v>
+      </c>
+      <c r="E73">
+        <v>0.08</v>
+      </c>
+      <c r="F73">
+        <v>0.07000000000000001</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -2028,6 +2118,18 @@
           <t>GoJu</t>
         </is>
       </c>
+      <c r="C84">
+        <v>0.14</v>
+      </c>
+      <c r="D84">
+        <v>0.15</v>
+      </c>
+      <c r="E84">
+        <v>0.1</v>
+      </c>
+      <c r="F84">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -2038,6 +2140,18 @@
           <t>StMi</t>
         </is>
       </c>
+      <c r="C85">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D85">
+        <v>0.09</v>
+      </c>
+      <c r="E85">
+        <v>0.39</v>
+      </c>
+      <c r="F85">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -2048,6 +2162,18 @@
           <t>SeFa</t>
         </is>
       </c>
+      <c r="C86">
+        <v>0.42</v>
+      </c>
+      <c r="D86">
+        <v>0.13</v>
+      </c>
+      <c r="E86">
+        <v>0.08</v>
+      </c>
+      <c r="F86">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -2058,6 +2184,18 @@
           <t>BIDA</t>
         </is>
       </c>
+      <c r="C87">
+        <v>0.34</v>
+      </c>
+      <c r="D87">
+        <v>0.21</v>
+      </c>
+      <c r="E87">
+        <v>0.34</v>
+      </c>
+      <c r="F87">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -2068,6 +2206,18 @@
           <t>DecBen</t>
         </is>
       </c>
+      <c r="C88">
+        <v>0.17</v>
+      </c>
+      <c r="D88">
+        <v>0.06</v>
+      </c>
+      <c r="E88">
+        <v>0.08</v>
+      </c>
+      <c r="F88">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -2078,6 +2228,18 @@
           <t>LFK</t>
         </is>
       </c>
+      <c r="C89">
+        <v>0.09</v>
+      </c>
+      <c r="D89">
+        <v>0.08</v>
+      </c>
+      <c r="E89">
+        <v>0.05</v>
+      </c>
+      <c r="F89">
+        <v>0.07000000000000001</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -2088,6 +2250,18 @@
           <t>GUDW</t>
         </is>
       </c>
+      <c r="C90">
+        <v>0.26</v>
+      </c>
+      <c r="D90">
+        <v>0.17</v>
+      </c>
+      <c r="E90">
+        <v>0.14</v>
+      </c>
+      <c r="F90">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -2098,6 +2272,18 @@
           <t>ANQU</t>
         </is>
       </c>
+      <c r="C91">
+        <v>0.37</v>
+      </c>
+      <c r="D91">
+        <v>0.23</v>
+      </c>
+      <c r="E91">
+        <v>0.2</v>
+      </c>
+      <c r="F91">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -2108,6 +2294,18 @@
           <t>HETH</t>
         </is>
       </c>
+      <c r="C92">
+        <v>0.13</v>
+      </c>
+      <c r="D92">
+        <v>0.15</v>
+      </c>
+      <c r="E92">
+        <v>0.15</v>
+      </c>
+      <c r="F92">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -2128,6 +2326,18 @@
           <t>ANPI</t>
         </is>
       </c>
+      <c r="C94">
+        <v>0.17</v>
+      </c>
+      <c r="D94">
+        <v>0.17</v>
+      </c>
+      <c r="E94">
+        <v>0.3</v>
+      </c>
+      <c r="F94">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -2202,6 +2412,18 @@
           <t>OLHA</t>
         </is>
       </c>
+      <c r="C99">
+        <v>0.36</v>
+      </c>
+      <c r="D99">
+        <v>0.49</v>
+      </c>
+      <c r="E99">
+        <v>0.97</v>
+      </c>
+      <c r="F99">
+        <v>0.87</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -2234,6 +2456,18 @@
           <t>ELSO</t>
         </is>
       </c>
+      <c r="C101">
+        <v>0.26</v>
+      </c>
+      <c r="D101">
+        <v>0.2</v>
+      </c>
+      <c r="E101">
+        <v>0.26</v>
+      </c>
+      <c r="F101">
+        <v>0.19</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -2244,6 +2478,18 @@
           <t>JELE</t>
         </is>
       </c>
+      <c r="C102">
+        <v>0.1</v>
+      </c>
+      <c r="D102">
+        <v>0.13</v>
+      </c>
+      <c r="E102">
+        <v>0.28</v>
+      </c>
+      <c r="F102">
+        <v>0.39</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -2254,6 +2500,18 @@
           <t>MACO</t>
         </is>
       </c>
+      <c r="C103">
+        <v>0.25</v>
+      </c>
+      <c r="D103">
+        <v>0.22</v>
+      </c>
+      <c r="E103">
+        <v>0.22</v>
+      </c>
+      <c r="F103">
+        <v>0.22</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -2286,6 +2544,18 @@
           <t>BOLE</t>
         </is>
       </c>
+      <c r="C105">
+        <v>0.16</v>
+      </c>
+      <c r="D105">
+        <v>0.15</v>
+      </c>
+      <c r="E105">
+        <v>0.12</v>
+      </c>
+      <c r="F105">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -2296,6 +2566,18 @@
           <t>LOIBAU</t>
         </is>
       </c>
+      <c r="C106">
+        <v>0.23</v>
+      </c>
+      <c r="D106">
+        <v>0.18</v>
+      </c>
+      <c r="E106">
+        <v>0.15</v>
+      </c>
+      <c r="F106">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -2416,6 +2698,18 @@
           <t>JERO</t>
         </is>
       </c>
+      <c r="C112">
+        <v>0.04</v>
+      </c>
+      <c r="D112">
+        <v>0.08</v>
+      </c>
+      <c r="E112">
+        <v>0.09</v>
+      </c>
+      <c r="F112">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -2586,6 +2880,18 @@
           <t>FLOND</t>
         </is>
       </c>
+      <c r="C123">
+        <v>0.17</v>
+      </c>
+      <c r="D123">
+        <v>0.25</v>
+      </c>
+      <c r="E123">
+        <v>0.21</v>
+      </c>
+      <c r="F123">
+        <v>0.19</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124">
@@ -2618,6 +2924,18 @@
           <t>LUMAR</t>
         </is>
       </c>
+      <c r="C125">
+        <v>0.17</v>
+      </c>
+      <c r="D125">
+        <v>0.17</v>
+      </c>
+      <c r="E125">
+        <v>0.18</v>
+      </c>
+      <c r="F125">
+        <v>0.14</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126">
@@ -2658,6 +2976,18 @@
           <t>POVI</t>
         </is>
       </c>
+      <c r="C129">
+        <v>0.05</v>
+      </c>
+      <c r="D129">
+        <v>0.17</v>
+      </c>
+      <c r="E129">
+        <v>0.02</v>
+      </c>
+      <c r="F129">
+        <v>0.24</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130">
@@ -2667,6 +2997,18 @@
         <is>
           <t>FRMA</t>
         </is>
+      </c>
+      <c r="C130">
+        <v>0.11</v>
+      </c>
+      <c r="D130">
+        <v>0.08</v>
+      </c>
+      <c r="E130">
+        <v>0.03</v>
+      </c>
+      <c r="F130">
+        <v>0.03</v>
       </c>
     </row>
     <row r="131">

</xml_diff>